<commit_message>
panel,header,login,inicio y varaibles nuevas
</commit_message>
<xml_diff>
--- a/php/vista/TEMP/BALANCE DE COMPROBACIÓN.xlsx
+++ b/php/vista/TEMP/BALANCE DE COMPROBACIÓN.xlsx
@@ -60,7 +60,7 @@
         <sz val="8"/>
         <u val="none"/>
       </rPr>
-      <t xml:space="preserve">00:29
+      <t xml:space="preserve">21:18
 </t>
     </r>
     <r>
@@ -85,7 +85,7 @@
         <sz val="8"/>
         <u val="none"/>
       </rPr>
-      <t xml:space="preserve">16-07-2021
+      <t xml:space="preserve">29-07-2021
 </t>
     </r>
     <r>
@@ -705,7 +705,7 @@
               <sz val="8"/>
               <u val="none"/>
             </rPr>
-            <t xml:space="preserve">00:29
+            <t xml:space="preserve">21:18
 </t>
           </r>
           <r>
@@ -730,7 +730,7 @@
               <sz val="8"/>
               <u val="none"/>
             </rPr>
-            <t xml:space="preserve">16-07-2021
+            <t xml:space="preserve">29-07-2021
 </t>
           </r>
           <r>

</xml_diff>